<commit_message>
The file weekdays.json was uodated
</commit_message>
<xml_diff>
--- a/templates/form_5.xlsx
+++ b/templates/form_5.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Рабочий стол\pdfProject\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\psolovey.GSN07\Desktop\auto\useful_functions\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -346,6 +346,9 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -376,19 +379,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="12">
     <dxf>
       <font>
         <b/>
         <i val="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -403,6 +410,51 @@
       </font>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF07676"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -410,6 +462,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF07676"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -722,174 +779,174 @@
       <c r="A3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="17"/>
-      <c r="V5" s="17"/>
-      <c r="W5" s="17"/>
-      <c r="X5" s="17"/>
-      <c r="Y5" s="17"/>
-      <c r="Z5" s="17"/>
-      <c r="AA5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="18"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="18"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="17"/>
-      <c r="V6" s="17"/>
-      <c r="W6" s="17"/>
-      <c r="X6" s="17"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="17"/>
-      <c r="AA6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="18"/>
+      <c r="AA6" s="18"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="18"/>
-      <c r="Z7" s="18"/>
-      <c r="AA7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="19"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="20"/>
-      <c r="U8" s="20"/>
-      <c r="V8" s="20"/>
-      <c r="W8" s="20"/>
-      <c r="X8" s="20"/>
-      <c r="Y8" s="20"/>
-      <c r="Z8" s="20"/>
-      <c r="AA8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="21"/>
+      <c r="Z8" s="21"/>
+      <c r="AA8" s="21"/>
     </row>
     <row r="10" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="15"/>
-      <c r="AA11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="16"/>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="17"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="5">
         <v>0</v>
       </c>
@@ -964,9 +1021,9 @@
       </c>
     </row>
     <row r="13" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="1" t="s">
         <v>7</v>
       </c>
@@ -1041,9 +1098,9 @@
       </c>
     </row>
     <row r="14" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="1" t="s">
         <v>3</v>
       </c>
@@ -2528,8 +2585,11 @@
     <mergeCell ref="B11:B14"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:D3">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>MIN($B3:$D3)=B3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="greaterThan">
+      <formula>0.2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2575,174 +2635,174 @@
       <c r="A3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="17"/>
-      <c r="V5" s="17"/>
-      <c r="W5" s="17"/>
-      <c r="X5" s="17"/>
-      <c r="Y5" s="17"/>
-      <c r="Z5" s="17"/>
-      <c r="AA5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="18"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="18"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="17"/>
-      <c r="V6" s="17"/>
-      <c r="W6" s="17"/>
-      <c r="X6" s="17"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="17"/>
-      <c r="AA6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="18"/>
+      <c r="AA6" s="18"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="18"/>
-      <c r="Z7" s="18"/>
-      <c r="AA7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="19"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="20"/>
-      <c r="U8" s="20"/>
-      <c r="V8" s="20"/>
-      <c r="W8" s="20"/>
-      <c r="X8" s="20"/>
-      <c r="Y8" s="20"/>
-      <c r="Z8" s="20"/>
-      <c r="AA8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="21"/>
+      <c r="Z8" s="21"/>
+      <c r="AA8" s="21"/>
     </row>
     <row r="10" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="15"/>
-      <c r="AA11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="16"/>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="17"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="5">
         <v>0</v>
       </c>
@@ -2817,9 +2877,9 @@
       </c>
     </row>
     <row r="13" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="1" t="s">
         <v>7</v>
       </c>
@@ -2894,9 +2954,9 @@
       </c>
     </row>
     <row r="14" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="1" t="s">
         <v>3</v>
       </c>
@@ -4381,8 +4441,11 @@
     <mergeCell ref="D11:AA11"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:D3">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>MIN($B3:$D3)=B3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+      <formula>0.2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4428,174 +4491,174 @@
       <c r="A3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="17"/>
-      <c r="V5" s="17"/>
-      <c r="W5" s="17"/>
-      <c r="X5" s="17"/>
-      <c r="Y5" s="17"/>
-      <c r="Z5" s="17"/>
-      <c r="AA5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="18"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="18"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="17"/>
-      <c r="V6" s="17"/>
-      <c r="W6" s="17"/>
-      <c r="X6" s="17"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="17"/>
-      <c r="AA6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="18"/>
+      <c r="AA6" s="18"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="18"/>
-      <c r="Z7" s="18"/>
-      <c r="AA7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="19"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="20"/>
-      <c r="U8" s="20"/>
-      <c r="V8" s="20"/>
-      <c r="W8" s="20"/>
-      <c r="X8" s="20"/>
-      <c r="Y8" s="20"/>
-      <c r="Z8" s="20"/>
-      <c r="AA8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="21"/>
+      <c r="Z8" s="21"/>
+      <c r="AA8" s="21"/>
     </row>
     <row r="10" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="15"/>
-      <c r="AA11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="16"/>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="17"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="5">
         <v>0</v>
       </c>
@@ -4670,9 +4733,9 @@
       </c>
     </row>
     <row r="13" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="1" t="s">
         <v>7</v>
       </c>
@@ -4747,9 +4810,9 @@
       </c>
     </row>
     <row r="14" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="1" t="s">
         <v>3</v>
       </c>
@@ -6234,8 +6297,11 @@
     <mergeCell ref="D11:AA11"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:D3">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>MIN($B3:$D3)=B3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+      <formula>0.2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6281,174 +6347,174 @@
       <c r="A3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="17"/>
-      <c r="U5" s="17"/>
-      <c r="V5" s="17"/>
-      <c r="W5" s="17"/>
-      <c r="X5" s="17"/>
-      <c r="Y5" s="17"/>
-      <c r="Z5" s="17"/>
-      <c r="AA5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="18"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="18"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="17"/>
-      <c r="V6" s="17"/>
-      <c r="W6" s="17"/>
-      <c r="X6" s="17"/>
-      <c r="Y6" s="17"/>
-      <c r="Z6" s="17"/>
-      <c r="AA6" s="17"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="18"/>
+      <c r="AA6" s="18"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="18"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="18"/>
-      <c r="Z7" s="18"/>
-      <c r="AA7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="19"/>
+      <c r="V7" s="19"/>
+      <c r="W7" s="19"/>
+      <c r="X7" s="19"/>
+      <c r="Y7" s="19"/>
+      <c r="Z7" s="19"/>
+      <c r="AA7" s="19"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="20"/>
-      <c r="M8" s="20"/>
-      <c r="N8" s="20"/>
-      <c r="O8" s="20"/>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="20"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="20"/>
-      <c r="U8" s="20"/>
-      <c r="V8" s="20"/>
-      <c r="W8" s="20"/>
-      <c r="X8" s="20"/>
-      <c r="Y8" s="20"/>
-      <c r="Z8" s="20"/>
-      <c r="AA8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="21"/>
+      <c r="V8" s="21"/>
+      <c r="W8" s="21"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="21"/>
+      <c r="Z8" s="21"/>
+      <c r="AA8" s="21"/>
     </row>
     <row r="10" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="15"/>
-      <c r="O11" s="15"/>
-      <c r="P11" s="15"/>
-      <c r="Q11" s="15"/>
-      <c r="R11" s="15"/>
-      <c r="S11" s="15"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="15"/>
-      <c r="X11" s="15"/>
-      <c r="Y11" s="15"/>
-      <c r="Z11" s="15"/>
-      <c r="AA11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="16"/>
+      <c r="V11" s="16"/>
+      <c r="W11" s="16"/>
+      <c r="X11" s="16"/>
+      <c r="Y11" s="16"/>
+      <c r="Z11" s="16"/>
+      <c r="AA11" s="17"/>
     </row>
     <row r="12" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="12"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
       <c r="D12" s="5">
         <v>0</v>
       </c>
@@ -6523,9 +6589,9 @@
       </c>
     </row>
     <row r="13" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="12"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
       <c r="D13" s="1" t="s">
         <v>7</v>
       </c>
@@ -6600,9 +6666,9 @@
       </c>
     </row>
     <row r="14" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
       <c r="D14" s="1" t="s">
         <v>3</v>
       </c>
@@ -8087,8 +8153,11 @@
     <mergeCell ref="D11:AA11"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:D3">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>MIN($B3:$D3)=B3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>0.2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>